<commit_message>
- Correções solicitadas no documento: ORDEM SERVIÇO E ORÇAMENTO 01122016
</commit_message>
<xml_diff>
--- a/storage/uploads/import/import_clientes.xlsx
+++ b/storage/uploads/import/import_clientes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\PROJETOS\WORKANA\06-16_SISTEMA_GESTÃO_ATLAS\IMPORTAÇÕES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\workana\gestaoatlas\storage\uploads\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3017,7 +3017,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="###,###,###,###"/>
+    <numFmt numFmtId="164" formatCode="###,###,###,###"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -3056,7 +3056,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3078,6 +3078,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFAFAE4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3109,7 +3115,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3127,16 +3133,20 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3477,10 +3487,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="L164" sqref="L164"/>
+      <selection pane="bottomLeft" activeCell="A114" sqref="A114:XFD114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3491,7 +3501,7 @@
     <col min="8" max="8" width="44.42578125" style="3" customWidth="1"/>
     <col min="9" max="9" width="12.28515625" style="9" customWidth="1"/>
     <col min="10" max="10" width="12.28515625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="27" style="3" customWidth="1"/>
     <col min="12" max="12" width="17.7109375" style="16" customWidth="1"/>
     <col min="13" max="13" width="19.28515625" style="3" customWidth="1"/>
     <col min="14" max="14" width="45" style="3" customWidth="1"/>
@@ -7482,38 +7492,38 @@
         <v>790</v>
       </c>
     </row>
-    <row r="114" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+    <row r="114" spans="1:33" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D114" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="E114" t="s">
-        <v>285</v>
-      </c>
-      <c r="F114" t="s">
+      <c r="E114" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="F114" s="17" t="s">
         <v>293</v>
       </c>
-      <c r="G114" t="s">
+      <c r="G114" s="17" t="s">
         <v>350</v>
       </c>
-      <c r="H114" t="s">
+      <c r="H114" s="17" t="s">
         <v>852</v>
       </c>
-      <c r="I114" s="9">
+      <c r="I114" s="19">
         <v>2021</v>
       </c>
-      <c r="K114" t="s">
+      <c r="K114" s="17" t="s">
         <v>551</v>
       </c>
-      <c r="L114" s="12" t="s">
+      <c r="L114" s="20" t="s">
         <v>599</v>
       </c>
-      <c r="N114" t="s">
+      <c r="N114" s="17" t="s">
         <v>654</v>
       </c>
-      <c r="AG114" t="s">
+      <c r="AG114" s="17" t="s">
         <v>791</v>
       </c>
     </row>
@@ -7800,38 +7810,38 @@
         <v>799</v>
       </c>
     </row>
-    <row r="123" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
+    <row r="123" spans="1:33" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D123" t="s">
+      <c r="D123" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="E123" t="s">
-        <v>285</v>
-      </c>
-      <c r="F123" t="s">
+      <c r="E123" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="F123" s="17" t="s">
         <v>288</v>
       </c>
-      <c r="G123" t="s">
+      <c r="G123" s="17" t="s">
         <v>351</v>
       </c>
-      <c r="H123" t="s">
+      <c r="H123" s="17" t="s">
         <v>948</v>
       </c>
-      <c r="I123" s="9">
+      <c r="I123" s="19">
         <v>2333</v>
       </c>
-      <c r="K123" t="s">
+      <c r="K123" s="17" t="s">
         <v>560</v>
       </c>
-      <c r="L123" s="12">
+      <c r="L123" s="20">
         <v>582876210111</v>
       </c>
-      <c r="N123" t="s">
+      <c r="N123" s="17" t="s">
         <v>654</v>
       </c>
-      <c r="AG123" t="s">
+      <c r="AG123" s="17" t="s">
         <v>800</v>
       </c>
     </row>

</xml_diff>